<commit_message>
Revert "github for win"
This reverts commit 7de21fceb78772ac6b06278ffe3c873746ea9996.
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>aaaa</t>
     <phoneticPr fontId="1"/>
@@ -27,10 +27,6 @@
   </si>
   <si>
     <t>dddd</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>github for win</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -378,7 +374,7 @@
   <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -399,8 +395,8 @@
       </c>
     </row>
     <row r="5" spans="2:2">
-      <c r="B5" t="s">
-        <v>3</v>
+      <c r="B5">
+        <v>2222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "github for win""
This reverts commit b62cc6d6d6a31deff5fcb79cc59af7a81918182f.
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>aaaa</t>
     <phoneticPr fontId="1"/>
@@ -27,6 +27,10 @@
   </si>
   <si>
     <t>dddd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>github for win</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -374,7 +378,7 @@
   <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -395,8 +399,8 @@
       </c>
     </row>
     <row r="5" spans="2:2">
-      <c r="B5">
-        <v>2222</v>
+      <c r="B5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>